<commit_message>
Generates all evals from a script
</commit_message>
<xml_diff>
--- a/Papers/Reference Manager.xlsx
+++ b/Papers/Reference Manager.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Desktop\Active_Constraints\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D04B5A5-361C-4012-B13B-1954718601E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BF51F-4FF9-42EC-99E7-76DCC5EABE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{04A67FA2-844F-4902-A542-C77338D125E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04A67FA2-844F-4902-A542-C77338D125E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
-    <sheet name="State of the Art" sheetId="3" r:id="rId2"/>
-    <sheet name="Materials and Methods" sheetId="5" r:id="rId3"/>
-    <sheet name="Experimental Protocol" sheetId="6" r:id="rId4"/>
-    <sheet name="Results and Discussion" sheetId="8" r:id="rId5"/>
+    <sheet name="Surgical Simulators" sheetId="9" r:id="rId2"/>
+    <sheet name="State of the Art" sheetId="13" r:id="rId3"/>
+    <sheet name="Materials and Methods" sheetId="14" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
   <si>
     <t>Title</t>
   </si>
@@ -104,19 +103,151 @@
     <t>Gomes</t>
   </si>
   <si>
-    <t>Towards Skill Transfer via Learning-Based Guidance in Human-Robot Interaction: An Application to Orthopaedic Surgical Drilling Skill</t>
-  </si>
-  <si>
-    <t>Zahedi</t>
-  </si>
-  <si>
     <t>Description of surgical robotic systems/companies in use, with pending approval or discontinued</t>
   </si>
   <si>
-    <t>Study on skill transfer without VFs</t>
-  </si>
-  <si>
     <t>Review of surgical systems in different areas of medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fundamentals of robotic surgery: A course of basic robotic surgery skills based upon a 14-society consensus template of outcomes measures and curriculum </t>
+  </si>
+  <si>
+    <t>Conference defining a standardized protocol for training surgical skills (psychomotor, cognitive, …)</t>
+  </si>
+  <si>
+    <t>Current status of robotic simulators in acquisition of robotic surgical skills</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Description of various surgical training simulator on the market. Nothing about experimental protocol</t>
+  </si>
+  <si>
+    <t>Bric</t>
+  </si>
+  <si>
+    <t>Current state of virtual reality simulation in robotic surgery training: a review</t>
+  </si>
+  <si>
+    <t>Description and validation of surgical training platforms from Intuitive - ROSS,dVTraininer, dVSS, SEP</t>
+  </si>
+  <si>
+    <t>Judkins</t>
+  </si>
+  <si>
+    <t>Objective evaluation of expert and novice performance during robotic surgical training tasks</t>
+  </si>
+  <si>
+    <t>Experimental study with training protocol and metrics - Not in a virtual environment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shi </t>
+  </si>
+  <si>
+    <t>Role of Visuohaptic Surgical Training Simulator in Resident Education of Orthopedic Surgery</t>
+  </si>
+  <si>
+    <t>Lin</t>
+  </si>
+  <si>
+    <t>Development and validation of a surgical training simulator with haptic feedback for learning bone-sawing skill</t>
+  </si>
+  <si>
+    <t>Experimental study of dental surgical training with haptic feedback simulator</t>
+  </si>
+  <si>
+    <t>Experimental study of orthopedic surgical skills - Nice protocol, no VFs7</t>
+  </si>
+  <si>
+    <t>Jimbo</t>
+  </si>
+  <si>
+    <t>A new innovative laparoscopic fundoplication training simulator with a surgical skill validation system</t>
+  </si>
+  <si>
+    <t>Experimental study on suturing skills - Descriptive experimental protocol, no VFs</t>
+  </si>
+  <si>
+    <t>Enayati</t>
+  </si>
+  <si>
+    <t>Haptics in Robot-Assisted Surgery Challenges and Benefits</t>
+  </si>
+  <si>
+    <t>Extensive review of Virtual Fixtures</t>
+  </si>
+  <si>
+    <t>Ren</t>
+  </si>
+  <si>
+    <t>Dynamic 3-D virtual fixtures for minimally invasive beating heart procedures</t>
+  </si>
+  <si>
+    <t>Abbot</t>
+  </si>
+  <si>
+    <t>Haptic Virtual Fixtures for Robot-Assisted Manipulation</t>
+  </si>
+  <si>
+    <t>VF design consideration in general, no specific VF</t>
+  </si>
+  <si>
+    <t>Surface Guidance VF - Beating heart procedures</t>
+  </si>
+  <si>
+    <t>Bettini</t>
+  </si>
+  <si>
+    <t>Vision-assisted control for manipulation using virtual fixtures</t>
+  </si>
+  <si>
+    <t>Cilinder and Cone guidance VF</t>
+  </si>
+  <si>
+    <t>Kathib</t>
+  </si>
+  <si>
+    <t>Real-Time Obstacle Avoidance for Manipulators and Mobile Robots</t>
+  </si>
+  <si>
+    <t>Very old obstacle-avoidance VF</t>
+  </si>
+  <si>
+    <t>Bowyer</t>
+  </si>
+  <si>
+    <t>Active constraints/virtual fixtures: A survey</t>
+  </si>
+  <si>
+    <t>PILOT PAPER</t>
+  </si>
+  <si>
+    <t>Robotic Assistance-as-Needed for Enhanced Visuomotor Learning in Surgical Robotics Training: An Experimental Study</t>
+  </si>
+  <si>
+    <t>Virtual Simulator with Trajectory Guidance VF and detailed experimental protocol - For surgical training</t>
+  </si>
+  <si>
+    <t>Xin</t>
+  </si>
+  <si>
+    <t>Laparoscopic surgery, perceptual limitations and force: A review</t>
+  </si>
+  <si>
+    <t>Lack of force feedback causes surgical errors and intraoperative injuries</t>
+  </si>
+  <si>
+    <t>Kapoort</t>
+  </si>
+  <si>
+    <t>A Constrained Optimization Approach to Virtual Fixtures for Multi-Handed Tasks</t>
+  </si>
+  <si>
+    <t>Experimental Study on the benefits of virtual fixtures</t>
   </si>
 </sst>
 </file>
@@ -236,17 +367,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -270,41 +397,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,130 +738,155 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E38CF-341E-4B18-91D8-203181FB871D}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17" style="6" customWidth="1"/>
-    <col min="2" max="2" width="89.5546875" style="24" customWidth="1"/>
-    <col min="3" max="3" width="9" style="7" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="15" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="17" style="4" customWidth="1"/>
+    <col min="2" max="2" width="89.5546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>2021</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>2020</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>25</v>
+      <c r="D3" s="11" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>2019</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>2022</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="5">
         <v>2001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="5">
         <v>2015</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>23</v>
+      <c r="D7" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="5">
         <v>2011</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D9" s="16"/>
+      <c r="A9" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2006</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2008</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -752,66 +895,188 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069109EE-967E-4CDB-B002-8A9AA241B5A5}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C018A9-1787-469D-A492-DFA4BDC4E312}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="20" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="9" style="21" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" style="23" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="19"/>
+    <col min="1" max="1" width="17" style="4" customWidth="1"/>
+    <col min="2" max="2" width="89.5546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="31.8" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="20" t="s">
-        <v>22</v>
+      <c r="A2" s="4" t="s">
+        <v>26</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="21">
-        <v>2019</v>
-      </c>
-      <c r="D2" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="22"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B3" s="14"/>
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2015</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B4" s="14"/>
+      <c r="A4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2016</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D9" s="12"/>
+      <c r="A5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2009</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2014</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2017</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -820,55 +1085,204 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34B3788-F87F-46DD-8CD7-C97B5569749A}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{670D059B-E02B-4115-B2DA-D5B00AD46DEF}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="9" style="7" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="17" style="4" customWidth="1"/>
+    <col min="2" max="2" width="89.5546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="14"/>
-      <c r="E2" s="11"/>
+    <row r="2" spans="1:5" ht="16.8" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="17">
+        <v>2014</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B3" s="14"/>
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2016</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="9"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B4" s="14"/>
+      <c r="A4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5">
+        <v>2008</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="14"/>
+      <c r="A5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5">
+        <v>2007</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2004</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1986</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="31.2" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D9" s="12"/>
+      <c r="B9" s="14"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" s="14"/>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" s="14"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="14"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" s="14"/>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="14"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" s="14"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" s="14"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4"/>
+      <c r="B18" s="14"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="14"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="4"/>
+      <c r="B20" s="14"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="8"/>
+    </row>
+    <row r="21" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
+      <c r="B21" s="14"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="4"/>
+      <c r="B22" s="14"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -877,43 +1291,43 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892D4E07-CBF7-4749-B593-7C2B9791DE5B}">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FFA2FCB-C76E-4F73-8D74-5D50455D2EC7}">
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="9" style="7" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="17" style="4" customWidth="1"/>
+    <col min="2" max="2" width="89.5546875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="9" style="5" customWidth="1"/>
+    <col min="4" max="4" width="90.21875" style="11" customWidth="1"/>
+    <col min="5" max="5" width="26.44140625" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.4">
       <c r="B2" s="14"/>
-      <c r="E2" s="11"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B3" s="14"/>
@@ -924,65 +1338,54 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="B5" s="14"/>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B6" s="14"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B7" s="14"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B8" s="14"/>
+    </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9" s="14"/>
       <c r="D9" s="12"/>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01BB0C2C-4180-44C4-B04A-C09F4159B7A5}">
-  <dimension ref="A1:E9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="23.88671875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="67.5546875" style="13" customWidth="1"/>
-    <col min="3" max="3" width="9" style="7" customWidth="1"/>
-    <col min="4" max="4" width="90.21875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" style="10" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="8" customFormat="1" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="16.2" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="14"/>
-      <c r="E2" s="11"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B3" s="14"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B4" s="14"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B5" s="14"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="D9" s="12"/>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B10" s="14"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B11" s="14"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B12" s="14"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B13" s="14"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B14" s="14"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B16" s="14"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B17" s="14"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B18" s="14"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B20" s="14"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
+      <c r="B21" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New user study document
</commit_message>
<xml_diff>
--- a/Papers/Reference Manager.xlsx
+++ b/Papers/Reference Manager.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Desktop\Active_Constraints\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773BF51F-4FF9-42EC-99E7-76DCC5EABE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C375409E-3801-4937-8AFA-5083308F9947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{04A67FA2-844F-4902-A542-C77338D125E4}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="73">
   <si>
     <t>Title</t>
   </si>
@@ -248,6 +248,15 @@
   </si>
   <si>
     <t>Experimental Study on the benefits of virtual fixtures</t>
+  </si>
+  <si>
+    <t>Goodrich</t>
+  </si>
+  <si>
+    <t>Human-robot interaction: A survey</t>
+  </si>
+  <si>
+    <t>Defines and reviews HRI</t>
   </si>
 </sst>
 </file>
@@ -384,7 +393,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -409,7 +418,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -738,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{784E38CF-341E-4B18-91D8-203181FB871D}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
@@ -886,6 +895,20 @@
       </c>
       <c r="D10" s="11" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="5">
+        <v>2007</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>